<commit_message>
Update to litdb_to_bib script
</commit_message>
<xml_diff>
--- a/lit/LitDatabase.xlsx
+++ b/lit/LitDatabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Dropbox\Grandfathering\lit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA906FC-6252-4A20-A5FF-DD1E66D57814}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA83E26-8B61-47CC-A7C8-ED5D2142F6EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vintage Regs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
   <si>
     <t>Empiric</t>
   </si>
@@ -185,10 +185,111 @@
     <t>Categorical vars:</t>
   </si>
   <si>
-    <t>... Environmental regulations that grandfather existing plants, by not holding them to the same strict standards as new plants, may have the unintended consequence of retarding new investment. By mandating that any new pollution sources meet strict pollution control standards, the rule may keep older facilities from scrapping and being replaced by newer ones.  If new plants are cleaner, then this effect may increase pollution in the short run. I develop a dynamic model of a facility’s decisions over scrapping and abatement, which depend on capital depreciation, profitability shocks, and environ- mental policy. Using data from fossil fuel fired boilers at electric power plants, I estimate the structural parameters of the model and assess the impact of grandfathering in the Clean Air Act on sulfur dioxide emissions. Counterfactual policy simulations show that an increase in the stringency of performance standards would have led to a decrease in investment in new boilers. However, this does not lead to increased emissions, since there is less investment in dirtier coal boilers as compared to relatively cleaner oil or natural gas boilers.</t>
-  </si>
-  <si>
     <t>This paper analyzes the effects of the New Source Review (NSR) environmental regulations on coal-fired electric power plants.  Regulations that grew out of the Clean Air Act of 1970 required new electric generating plants to install costly SO2 control equipment but exempted existing plants.  Plants lost their exemptions if they made "major modifications."  By mandating that existing pollution sources meet strict pollution control standards, the rule may encourage older facilities to take costly steps to avoid meeting the new standards.  The authors examine whether this caused firms to invest less in grandfathered plants, possibly leading to lower efficiency and higher emissions.  Their paper focuses on how NSR affected inputs at "vulnerable" plants, that is grandfathered plants proxied by those without a scrubber.  They find evidence that heightened NSR enforcement over the 1998-2002 period reduced capital investment at vulnerable plants.  However, they find no discernible effect on other inputs or emissions.</t>
+  </si>
+  <si>
+    <t>... Environmental regulations that grandfather existing plants, by not holding them to the same strict standards as new plants, may have the unintended consequence of retarding new investment. By mandating that any new pollution sources meet strict pollution control standards, the rule may keep older facilities from scrapping and being replaced by newer ones.  If new plants are cleaner, then this effect may increase pollution in the short run. I develop a dynamic model of a facility’s decisions over scrapping and abatement, which depend on capital depreciation, profitability shocks, and environ- mental policy. Using data from fossil fuel fired boilers at electric power plants, I estimate the structural parameters of the model and assess the impact of grandfathering in the Clean Air Act on sulfur dioxide emissions. Counterfactual policy simulations show that an increase in the stringency of performance standards would have led to a decrease in investment in new boilers. However, this does not lead to increased emissions, since there is less investment in dirtier coal boilers as compared to relatively cleaner oil or natural gas boilers.
+... The purpose of this paper is to determine how grandfathering provisions in environmental policy affect both investment in and pollution from fossil fuel fired electric power plants. I develop a dynamic model of each facility’s decisions about investment in new capital and choice of abatement techniques. These decisions are affected by the relative profitability of new capital, the costs of upgrading, and environmental regulations. Newer capital pollutes less, and hence stricter environmental policy without grandfathering provides an extra incentive to upgrade. Yet stricter environmental policy with grandfathering may provide a disincentive to upgrade. Using data from 1985 to 1995 on U.S. electric power plants, I estimate the parameters of the model. Finally, I simulate the estimated model to determine how grandfathering in the CAA impacts emissions and investment.</t>
+  </si>
+  <si>
+    <t>Gruenspecht, H</t>
+  </si>
+  <si>
+    <t>Differentiated regulation: The case of auto emissions standards</t>
+  </si>
+  <si>
+    <t>81(3): 328-331</t>
+  </si>
+  <si>
+    <t>Nelson, R; Tietenberg, T; Donihue, M</t>
+  </si>
+  <si>
+    <t>Review of Economics and Statistics</t>
+  </si>
+  <si>
+    <t>Differential environmental regulation: Effects on electric utility capital turnover and emissions</t>
+  </si>
+  <si>
+    <t>75(2): 368-373</t>
+  </si>
+  <si>
+    <t>Levinson, A</t>
+  </si>
+  <si>
+    <t>Grandfather regulations, new source bias, and state air toxics regulations</t>
+  </si>
+  <si>
+    <t>Ecological Economics</t>
+  </si>
+  <si>
+    <t>28(2): 299-311</t>
+  </si>
+  <si>
+    <t>Maloney, M; Brady, G</t>
+  </si>
+  <si>
+    <t>Capital turnover and marketable pollution rights</t>
+  </si>
+  <si>
+    <t>Journal of Law and Economics</t>
+  </si>
+  <si>
+    <t>31(1): 203-226</t>
+  </si>
+  <si>
+    <t>List, J; Millimet, D; McHone, W</t>
+  </si>
+  <si>
+    <t>Advances in Economic Analysis and Policy</t>
+  </si>
+  <si>
+    <t>The unintended disincentive in the Clean Air Act</t>
+  </si>
+  <si>
+    <t>… An early examination of a grandfathered environmental policy, the author looks not at stationary air pollution sources but at automobiles. He finds that stricter vehicle emissions standards, which apply only to new cars and hence effectively grandfather old cars, lead to a perverse short-term increase in emissions.</t>
+  </si>
+  <si>
+    <t>… The authors find that environmental regulations increase the age of capital but not the level of emissions for electric utilities.</t>
+  </si>
+  <si>
+    <t>… The author finds no significant difference in capital vintage between states with and without grandfather provisions for manufacturing plants in commercial printing and paint manufacturing.</t>
+  </si>
+  <si>
+    <t>… The authors find perverse effects of grandfathering in the electric power industry.</t>
+  </si>
+  <si>
+    <t>… The authors find perverse effects of grandfathering in manufacturing plants in NY.</t>
+  </si>
+  <si>
+    <t>Bush v. Gore and the effect of New Source Review
+on power plant emissions</t>
+  </si>
+  <si>
+    <t>Lange, I; Linn, J</t>
+  </si>
+  <si>
+    <t>40(4): 571-591</t>
+  </si>
+  <si>
+    <t>Plant vintage, technology, and environmental regulation</t>
+  </si>
+  <si>
+    <t>Gray, WB; Shadbegian, RJ</t>
+  </si>
+  <si>
+    <t>Environmental and Resource Economics</t>
+  </si>
+  <si>
+    <t>46(3): 384-402</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Vehicles</t>
+  </si>
+  <si>
+    <t>4(2)</t>
   </si>
 </sst>
 </file>
@@ -269,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -309,6 +410,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,9 +616,45 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -679,45 +837,9 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -740,28 +862,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:L3" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:L10" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:L10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Pub" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Author(s)" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Year" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Title" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Journal/Organization" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Number" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Location" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Subject" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Method" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Data" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Summary" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Pub" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Author(s)" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Year" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Title" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Journal/Organization" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Number" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Location" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Subject" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Method" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Data" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Summary" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table143" displayName="Table143" ref="A1:L3" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table143" displayName="Table143" ref="A1:L3" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:L3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L3">
     <sortCondition ref="C2:C3"/>
@@ -769,18 +891,18 @@
     <sortCondition ref="E2:E3"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Pub" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Author(s)" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Year" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Title" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Journal/Organization" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Number" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Location" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Subject" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Method" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Data" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Summary" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Pub" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Author(s)" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Year" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Title" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Journal/Organization" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Number" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Location" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Subject" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Method" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Data" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Summary" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1107,12 +1229,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B40" sqref="B40"/>
-      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,10 +1324,10 @@
         <v>41</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="153" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1238,8 +1360,210 @@
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="2" t="s">
-        <v>50</v>
-      </c>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="51" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="20">
+        <v>1982</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1993</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="20">
+        <v>1999</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="20">
+        <v>1988</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="20">
+        <v>2004</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="23">
+        <v>2008</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+    </row>
+    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="23">
+        <v>2003</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Draft note to committee
</commit_message>
<xml_diff>
--- a/lit/LitDatabase.xlsx
+++ b/lit/LitDatabase.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Dropbox\Grandfathering\lit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7DF5F2-94E0-45D9-AB0C-F2A395ECD4CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3D3E3C-D26D-4D96-9D4A-7076613C6A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vintage Regs" sheetId="1" r:id="rId1"/>
-    <sheet name="Methods" sheetId="3" r:id="rId2"/>
+    <sheet name="Methods" sheetId="4" r:id="rId2"/>
     <sheet name="Notes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="204">
   <si>
     <t>Empiric</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Classified as to download</t>
   </si>
   <si>
-    <t>Electricity</t>
-  </si>
-  <si>
     <t>Abraham, S; Sun, L</t>
   </si>
   <si>
@@ -126,18 +123,6 @@
   </si>
   <si>
     <t>Event Study</t>
-  </si>
-  <si>
-    <t>Allcott, H; Rogers, T</t>
-  </si>
-  <si>
-    <t>The short-run and long-run effects of behavioral interventions: Experimental evidence from energy conservation</t>
-  </si>
-  <si>
-    <t>104(10): 3003-3037</t>
-  </si>
-  <si>
-    <t>… Paper which investigates social nudges through HERs and includes a panel fixed effects empirical strategy with weather variables.</t>
   </si>
   <si>
     <t>... NB -- Constituent of a recent literature exploring properties (and failures) of the two-way fixed effects estimator under heterogeneous causal effects.  Recent and emerging literature on heterogeneous treatment effects in DD with variation in treatment timing.</t>
@@ -288,9 +273,6 @@
     <t>Dynamic Structural Model; Simulation</t>
   </si>
   <si>
-    <t>Keohane,N ; Mansur, E; Voynuv, A</t>
-  </si>
-  <si>
     <t>Averting regulatory enforcement: Evidence from new source review</t>
   </si>
   <si>
@@ -434,6 +416,241 @@
   </si>
   <si>
     <t>Nash, JR; Revesz, RL</t>
+  </si>
+  <si>
+    <t>SA - Binary Choice</t>
+  </si>
+  <si>
+    <t>Divorce</t>
+  </si>
+  <si>
+    <t>82(1): 110-130</t>
+  </si>
+  <si>
+    <t>Journal of Economic Behavior and Organization</t>
+  </si>
+  <si>
+    <t>You can’t be happier than your wife. Happiness gaps and divorce</t>
+  </si>
+  <si>
+    <t>Guven, C; Senik, C; Stichnoth, H</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 42(4); 1260-1288</t>
+  </si>
+  <si>
+    <t>American Journal of Political Science</t>
+  </si>
+  <si>
+    <t>Taking time seriously: Time-series-cross-section analysis with a binary dependent variable</t>
+  </si>
+  <si>
+    <t>Beck, N; Katz, JN; Tucker, R</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>81(5): 2033-2053</t>
+  </si>
+  <si>
+    <t>Econometrica</t>
+  </si>
+  <si>
+    <t>Revolt on the Nile: Economic shocks, religion, and political power</t>
+  </si>
+  <si>
+    <t>Chaney, E</t>
+  </si>
+  <si>
+    <t>5(1): 129-138</t>
+  </si>
+  <si>
+    <t>Oxford Bulletin of Economics and Statistics</t>
+  </si>
+  <si>
+    <t>Easy estimation methods for discrete-time duration models</t>
+  </si>
+  <si>
+    <t>Jenkins, SP</t>
+  </si>
+  <si>
+    <t>10(4): 411-431</t>
+  </si>
+  <si>
+    <t>Journal of Applied Econometrics</t>
+  </si>
+  <si>
+    <t>A class of binary response models for grouped duration data</t>
+  </si>
+  <si>
+    <t>Sueyoshi, GT</t>
+  </si>
+  <si>
+    <t>18(2): 155-195</t>
+  </si>
+  <si>
+    <t>Journal of Educational Statistics</t>
+  </si>
+  <si>
+    <t>It’s about time: Using Discrete-time Survival Analysis to Study Duration and the Timing of Events</t>
+  </si>
+  <si>
+    <t>Singer, J; Willet, J</t>
+  </si>
+  <si>
+    <t>DD; SA - Binary Choice</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>102: 102336</t>
+  </si>
+  <si>
+    <t>Costs of inefficient regulation: Evidence from the Bakken</t>
+  </si>
+  <si>
+    <t>Lade, G; Rudik, I</t>
+  </si>
+  <si>
+    <t>DD - Multiple Periods</t>
+  </si>
+  <si>
+    <t>Working Paper; 25018; September</t>
+  </si>
+  <si>
+    <t>National Bureau of Economic Research</t>
+  </si>
+  <si>
+    <t>Difference-in-Differences with Variation in Treatment Timing</t>
+  </si>
+  <si>
+    <t>Goodman-Bacon, A</t>
+  </si>
+  <si>
+    <t>… The inconsistency of FE estimators for the average treatment effect in the presence of unit-specific response heterogeneity is well-established in the literature and has been documented in numerous studies (e.g., Gibbons, Serrato, and Urbancic, 2019; de Chaisemartin and d’Haultfoeuille, 2019).
+... The inconsistency of (one-way) fixed effects estimators in the presence of response heterogeneity and its convergence to a variance-weighted average of the heterogeneous parameters was shown in Chernozhukov et al. (2013) and its empirical relevance clearly illustrated in Gibbons, Serrato, and Urbancic (2019).</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>8(1): 1-12</t>
+  </si>
+  <si>
+    <t>Journal of Econometric Methods</t>
+  </si>
+  <si>
+    <t>Broken or fixed effects?</t>
+  </si>
+  <si>
+    <t>Gibbons, CE; Serrato, JCS; Urbancic, MB</t>
+  </si>
+  <si>
+    <t>DD - Multiple Treats</t>
+  </si>
+  <si>
+    <t>79(3): 426-433</t>
+  </si>
+  <si>
+    <t>Identification based on difference-in-differences approaches with multiple treatments</t>
+  </si>
+  <si>
+    <t>Fricke, H</t>
+  </si>
+  <si>
+    <t>... NB -- Constituent of a recent literature exploring properties (and failures) of the two-way fixed effects estimator under heterogeneous causal effects.
+… The inconsistency of FE estimators for the average treatment effect in the presence of unit-specific response heterogeneity is well-established in the literature and has been documented in numerous studies (e.g., Gibbons, Serrato, and Urbancic, 2019; de Chaisemartin and d’Haultfoeuille, 2019).
+... The properties of two-way fixed effects estimators have been examined in recent work (de Chaisemartin and d’Haultfoeuille, 2019; Callaway and Sant’Anna, 2019).</t>
+  </si>
+  <si>
+    <t>110(9):  2964-2996</t>
+  </si>
+  <si>
+    <t>Two-way fixed effects estimators with heterogeneous treatment effects</t>
+  </si>
+  <si>
+    <t>de Chaisemartin, C; d'Haultfoeuille, X</t>
+  </si>
+  <si>
+    <t>... NB -- Constituent of a recent literature exploring properties (and failures) of the two-way fixed effects estimator under heterogeneous causal effects.  Recent and emerging literature on heterogeneous treatment effects in DD with variation in treatment timing.
+... The properties of two-way fixed effects estimators have been examined in recent work (de Chaisemartin and d’Haultfoeuille, 2019; Callaway and Sant’Anna, 2019).</t>
+  </si>
+  <si>
+    <t>Working Paper; August</t>
+  </si>
+  <si>
+    <t>Social Science Research Network</t>
+  </si>
+  <si>
+    <t>Difference-in-Differences with Multiple Time Periods</t>
+  </si>
+  <si>
+    <t>Callaway, B; Sant'Anna, PHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working Paper; May </t>
+  </si>
+  <si>
+    <t>Revisiting Event Study Designs, with an Application to the Estimation of the Marginal Propensity to Consume</t>
+  </si>
+  <si>
+    <t>Borusyak, K; Jaravel, X</t>
+  </si>
+  <si>
+    <t>Working Paper; 24963; August</t>
+  </si>
+  <si>
+    <t>Design-based Analysis in Difference-in-Differences Settings with Staggered Adoption</t>
+  </si>
+  <si>
+    <t>Athley, S; Imbens, GW</t>
+  </si>
+  <si>
+    <t>Greenstone, M</t>
+  </si>
+  <si>
+    <t>The impacts of environmental regulations on industrial activity: Evidence from the 1970 and 1977 Clean Air Act Amendments and the Census of Manufactures</t>
+  </si>
+  <si>
+    <t>Journal of Political Economy</t>
+  </si>
+  <si>
+    <t>110(6): 1175-1219</t>
+  </si>
+  <si>
+    <t>Air Quality</t>
+  </si>
+  <si>
+    <t>Efficiency advantages of grandfathering in rights-based risheries management</t>
+  </si>
+  <si>
+    <t>Annual Review of Resource Economics</t>
+  </si>
+  <si>
+    <t>3(): 159-179</t>
+  </si>
+  <si>
+    <t>Anderson, T; Arnason, R; Libecap, GD</t>
+  </si>
+  <si>
+    <t>Working Paper; February</t>
+  </si>
+  <si>
+    <t>Regulatory avoidance and spillover: The effects of environmental regulation on emissions at coal-fired power plants</t>
+  </si>
+  <si>
+    <t>Raff, Z; Walter, JM</t>
+  </si>
+  <si>
+    <t>75(3): 378-420</t>
+  </si>
+  <si>
+    <t>Keohane,N ; Mansur, E; Voynov, A</t>
   </si>
 </sst>
 </file>
@@ -514,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -528,7 +745,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -561,6 +777,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -994,8 +1219,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:L23" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:L23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:L25" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:L25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L23">
     <sortCondition ref="C2:C23"/>
     <sortCondition ref="D2:D23"/>
@@ -1020,26 +1245,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table143" displayName="Table143" ref="A1:L3" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L3">
-    <sortCondition ref="C2:C3"/>
-    <sortCondition ref="D2:D3"/>
-    <sortCondition ref="E2:E3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0B9B4577-4218-46F2-A61F-FC70544A1FFD}" name="Table143" displayName="Table143" ref="A1:L17" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L9">
+    <sortCondition ref="C2:C9"/>
+    <sortCondition ref="D2:D9"/>
+    <sortCondition ref="E2:E9"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Pub" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Author(s)" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Year" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Title" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Journal/Organization" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Number" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Location" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Subject" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Method" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Data" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="Summary" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E4FA0306-FCF5-45E6-AA26-BA2FE291733F}" name="Pub" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E9A7319A-42BE-42DC-BB52-7F99A9C86A4A}" name="Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{91A66D3C-4DA6-4126-807F-99B47519E4CF}" name="Author(s)" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{AE8D30E4-A9F9-429C-A204-024A93D95551}" name="Year" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{B7D1B4C4-BF6A-477E-9414-7F44A3A90D38}" name="Title" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{7D24037F-DA0E-426A-85A4-057EF01965BE}" name="Journal/Organization" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{BAAB9BED-FE35-468B-8023-566E0F0DE996}" name="Number" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{05B76D40-7ED5-451F-BF34-E26926D0EA27}" name="Location" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{730DBE6A-DD02-4EEA-81A1-00168B3DDF50}" name="Subject" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{92FF14B4-CD71-42DA-99DF-0199F7AC31BD}" name="Method" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{D938D87D-4F7B-45DE-AEB0-55271AADDFEB}" name="Data" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{BFA62ED2-7AEE-4516-B242-6574B9B7AE2B}" name="Summary" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1366,12 +1591,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B40" sqref="B40"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,95 +1613,95 @@
     <col min="12" max="12" width="80.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="14">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="13">
         <v>1999</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="E2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="14">
+      <c r="A3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="13">
         <v>2005</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="E3" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1486,191 +1711,193 @@
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4">
         <v>2012</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14" t="s">
+      <c r="A5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="13">
+        <v>2011</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2020</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+    </row>
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="14">
-        <v>2011</v>
-      </c>
-      <c r="E5" s="14" t="s">
+      <c r="D7" s="13">
+        <v>2019</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="G5" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-    </row>
-    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="19">
-        <v>2020</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="G7" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-    </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="19">
-        <v>2019</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="19">
+      <c r="A8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="13">
         <v>2003</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1982</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-    </row>
-    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="14">
-        <v>1982</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="18" t="s">
-        <v>68</v>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="17" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="14">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="13">
         <v>2007</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="E10" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:12" ht="204" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1680,363 +1907,415 @@
         <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D11" s="4">
         <v>2011</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" s="18">
+        <v>2009</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="18">
+        <v>2008</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+    </row>
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1999</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="13">
+        <v>2004</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="13">
+        <v>1988</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="11">
+        <v>2007</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="G17" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="19">
-        <v>2009</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-    </row>
-    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="19">
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+    </row>
+    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="13">
+        <v>1993</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2011</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="11">
+        <v>2018</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+    </row>
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="22">
         <v>2008</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E21" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+    </row>
+    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="13">
+        <v>1993</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="18">
+        <v>2006</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+    </row>
+    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24" s="11">
+        <v>2011</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+    </row>
+    <row r="25" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D25" s="13">
+        <v>2020</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F25" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-    </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="14">
-        <v>1999</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="14">
-        <v>2004</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="19">
-        <v>1988</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="12">
-        <v>2007</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-    </row>
-    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="14">
-        <v>1993</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D19" s="12">
-        <v>2011</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-    </row>
-    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="12">
-        <v>2018</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-    </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D21" s="12">
-        <v>2008</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-    </row>
-    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="14">
-        <v>1993</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-    </row>
-    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D23" s="19">
-        <v>2006</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
+      <c r="G25" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2048,13 +2327,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E37B5B6-B000-4D2C-BCAC-21988B96F2A7}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B40" sqref="B40"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2072,109 +2351,545 @@
     <col min="12" max="12" width="80.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="18">
+        <v>2020</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="14">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="18">
+        <v>2018</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="18">
+        <v>2017</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="18">
         <v>2020</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15" t="s">
+      <c r="E5" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2020</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="K6" s="20"/>
+      <c r="L6" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="13">
+        <v>2017</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" spans="1:12" ht="102" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="18">
+        <v>2018</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2018</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="L9" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C10" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2020</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="12">
-        <v>2014</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G10" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="H10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13" t="s">
-        <v>34</v>
-      </c>
+      <c r="I10" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+    </row>
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1993</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="13">
+        <v>1995</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1995</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="11">
+        <v>2012</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" s="13">
+        <v>1998</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="11">
+        <v>2012</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+    </row>
+    <row r="17" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="11">
+        <v>2002</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2196,11 +2911,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2208,32 +2923,32 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2241,25 +2956,25 @@
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>48</v>
+      <c r="B9" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
-        <v>46</v>
+      <c r="B10" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
-        <v>47</v>
+      <c r="B11" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>